<commit_message>
added the new fig 1 and 2
</commit_message>
<xml_diff>
--- a/result/execution_times.xlsx
+++ b/result/execution_times.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
   <si>
     <t xml:space="preserve">ml_method</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">text-mining</t>
   </si>
   <si>
-    <t xml:space="preserve">cor-5000</t>
+    <t xml:space="preserve">cor-500</t>
   </si>
   <si>
     <t xml:space="preserve">var-100</t>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">DL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cor-500</t>
   </si>
 </sst>
 </file>
@@ -79,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,8 +142,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,248 +280,281 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>2514.373752</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>5807.536423</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>10754.97132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="2" t="n">
+        <v>3411.4386</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="2" t="n">
+        <v>2693.9418</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="2" t="n">
+        <v>2693.9418</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C9" s="2" t="n">
+        <v>3553.4004</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C10" s="2" t="n">
+        <v>3411.4386</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>3452.060023</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>286.5259821</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="0" t="s">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>6590.61241</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C14" s="2" t="n">
+        <v>121.6083</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C15" s="2" t="n">
+        <v>76.89216</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C16" s="2" t="n">
+        <v>61.52664</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C17" s="2" t="n">
+        <v>78.564</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C18" s="2" t="n">
+        <v>74.66988</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C19" s="2" t="n">
+        <v>93.49674</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="0" t="n">
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>5483.367728</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>3393.934803</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>2306.136289</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>1983.89089</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>2162.181644</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>2460.712538</v>
       </c>
     </row>

</xml_diff>